<commit_message>
Added Products to Items
</commit_message>
<xml_diff>
--- a/Deployment/ItemAuto.xlsx
+++ b/Deployment/ItemAuto.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawantsp1\trail\DataHub\Deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawantsp1\Hub\DataHub\Deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC21030-EDDC-404A-8162-A3709A23A90F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5943BC-CD7A-4B4B-9071-5F1C2B2D3009}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9F09ADC-1856-4E8A-9013-6B506ECF6396}"/>
   </bookViews>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B4FBB80-8DBE-4456-8A5E-26FFAB1127D9}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -452,6 +452,23 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>